<commit_message>
realizadas todas las correcciones, sigue convertirlo en exe, probarlo y luego empezar con el proyecto django
</commit_message>
<xml_diff>
--- a/3.xlsx
+++ b/3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intralogargentinasa-my.sharepoint.com/personal/ftorres_intralog_com_ar/Documents/APIS/API_Wordpess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6FB5368F5B205C37F3383C11595ED87656CF0357" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14CF2EB1-E766-4665-9F8B-E4B42E8E7187}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_6FB5368F5B205C37F3383C11595ED87656CF0357" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{723EAFC4-6E45-4988-9FEF-42573A13CAD7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2782,7 +2782,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2794,6 +2794,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2831,9 +2838,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3140,7 +3150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3164,7 +3176,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">

</xml_diff>